<commit_message>
Tables 4 and 5
</commit_message>
<xml_diff>
--- a/Table4_Terrestrial.xlsx
+++ b/Table4_Terrestrial.xlsx
@@ -12,18 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area_Sq_Km</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion</t>
   </si>
   <si>
-    <t xml:space="preserve">Samlet</t>
+    <t xml:space="preserve">Skov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sø</t>
   </si>
   <si>
     <t xml:space="preserve">Habitatnaturtype</t>
@@ -32,7 +38,7 @@
     <t xml:space="preserve">Saerligt</t>
   </si>
   <si>
-    <t xml:space="preserve">Pleje og graes</t>
+    <t xml:space="preserve">Pleje_og_graes</t>
   </si>
   <si>
     <t xml:space="preserve">Stoette</t>
@@ -377,60 +383,114 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>3878.6247</v>
       </c>
       <c r="C2" t="n">
         <v>8.98977509902045</v>
+      </c>
+      <c r="D2" t="n">
+        <v>992.738</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1483.7534</v>
+      </c>
+      <c r="F2" t="n">
+        <v>355.642</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>1755.2573</v>
       </c>
       <c r="C3" t="n">
         <v>4.0682895583875</v>
+      </c>
+      <c r="D3" t="n">
+        <v>329.4762</v>
+      </c>
+      <c r="E3" t="n">
+        <v>952.1239</v>
+      </c>
+      <c r="F3" t="n">
+        <v>323.0868</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="n">
         <v>1537.0693</v>
       </c>
       <c r="C4" t="n">
         <v>3.56257910661189</v>
+      </c>
+      <c r="D4" t="n">
+        <v>76.3708</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1249.1788</v>
+      </c>
+      <c r="F4" t="n">
+        <v>39.4313</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
         <v>595.9982</v>
       </c>
       <c r="C5" t="n">
         <v>1.38138907263211</v>
+      </c>
+      <c r="D5" t="n">
+        <v>13.79</v>
+      </c>
+      <c r="E5" t="n">
+        <v>499.8937</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0893</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
         <v>32.8415</v>
       </c>
       <c r="C6" t="n">
         <v>0.0761191715492556</v>
+      </c>
+      <c r="D6" t="n">
+        <v>23.6622</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8.674</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>